<commit_message>
Feed data, process updated
</commit_message>
<xml_diff>
--- a/process/Iteration01.xlsx
+++ b/process/Iteration01.xlsx
@@ -154,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +182,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -225,6 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -646,7 +653,7 @@
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -669,7 +676,7 @@
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="11" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>